<commit_message>
Stats from previous weeks can be used to avoid recalculation
</commit_message>
<xml_diff>
--- a/totalGames.xlsx
+++ b/totalGames.xlsx
@@ -359,7 +359,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N15"/>
+  <dimension ref="A1:S15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -430,6 +430,31 @@
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
+          <t>Week13</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Week14</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Week15</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Week16</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Week17</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
           <t>Total</t>
         </is>
       </c>
@@ -477,7 +502,22 @@
         <v>34</v>
       </c>
       <c r="N2" t="n">
-        <v>389</v>
+        <v>33</v>
+      </c>
+      <c r="O2" t="n">
+        <v>34</v>
+      </c>
+      <c r="P2" t="n">
+        <v>27</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>34</v>
+      </c>
+      <c r="R2" t="n">
+        <v>5</v>
+      </c>
+      <c r="S2" t="n">
+        <v>522</v>
       </c>
     </row>
     <row r="3">
@@ -523,7 +563,22 @@
         <v>27</v>
       </c>
       <c r="N3" t="n">
-        <v>357</v>
+        <v>27</v>
+      </c>
+      <c r="O3" t="n">
+        <v>31</v>
+      </c>
+      <c r="P3" t="n">
+        <v>22</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>32</v>
+      </c>
+      <c r="R3" t="n">
+        <v>3</v>
+      </c>
+      <c r="S3" t="n">
+        <v>472</v>
       </c>
     </row>
     <row r="4">
@@ -569,7 +624,22 @@
         <v>29</v>
       </c>
       <c r="N4" t="n">
-        <v>370</v>
+        <v>24</v>
+      </c>
+      <c r="O4" t="n">
+        <v>30</v>
+      </c>
+      <c r="P4" t="n">
+        <v>26</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>31</v>
+      </c>
+      <c r="R4" t="n">
+        <v>7</v>
+      </c>
+      <c r="S4" t="n">
+        <v>488</v>
       </c>
     </row>
     <row r="5">
@@ -615,7 +685,22 @@
         <v>32</v>
       </c>
       <c r="N5" t="n">
-        <v>361</v>
+        <v>29</v>
+      </c>
+      <c r="O5" t="n">
+        <v>33</v>
+      </c>
+      <c r="P5" t="n">
+        <v>26</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>26</v>
+      </c>
+      <c r="R5" t="n">
+        <v>6</v>
+      </c>
+      <c r="S5" t="n">
+        <v>481</v>
       </c>
     </row>
     <row r="6">
@@ -661,7 +746,22 @@
         <v>26</v>
       </c>
       <c r="N6" t="n">
-        <v>352</v>
+        <v>32</v>
+      </c>
+      <c r="O6" t="n">
+        <v>32</v>
+      </c>
+      <c r="P6" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>26</v>
+      </c>
+      <c r="R6" t="n">
+        <v>6</v>
+      </c>
+      <c r="S6" t="n">
+        <v>478</v>
       </c>
     </row>
     <row r="7">
@@ -707,7 +807,22 @@
         <v>27</v>
       </c>
       <c r="N7" t="n">
-        <v>359</v>
+        <v>34</v>
+      </c>
+      <c r="O7" t="n">
+        <v>39</v>
+      </c>
+      <c r="P7" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>28</v>
+      </c>
+      <c r="R7" t="n">
+        <v>4</v>
+      </c>
+      <c r="S7" t="n">
+        <v>497</v>
       </c>
     </row>
     <row r="8">
@@ -753,7 +868,22 @@
         <v>33</v>
       </c>
       <c r="N8" t="n">
-        <v>388</v>
+        <v>33</v>
+      </c>
+      <c r="O8" t="n">
+        <v>33</v>
+      </c>
+      <c r="P8" t="n">
+        <v>26</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>38</v>
+      </c>
+      <c r="R8" t="n">
+        <v>4</v>
+      </c>
+      <c r="S8" t="n">
+        <v>522</v>
       </c>
     </row>
     <row r="9">
@@ -799,7 +929,22 @@
         <v>35</v>
       </c>
       <c r="N9" t="n">
-        <v>360</v>
+        <v>31</v>
+      </c>
+      <c r="O9" t="n">
+        <v>35</v>
+      </c>
+      <c r="P9" t="n">
+        <v>28</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>28</v>
+      </c>
+      <c r="R9" t="n">
+        <v>6</v>
+      </c>
+      <c r="S9" t="n">
+        <v>488</v>
       </c>
     </row>
     <row r="10">
@@ -845,7 +990,22 @@
         <v>21</v>
       </c>
       <c r="N10" t="n">
-        <v>308</v>
+        <v>21</v>
+      </c>
+      <c r="O10" t="n">
+        <v>25</v>
+      </c>
+      <c r="P10" t="n">
+        <v>16</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>15</v>
+      </c>
+      <c r="R10" t="n">
+        <v>2</v>
+      </c>
+      <c r="S10" t="n">
+        <v>387</v>
       </c>
     </row>
     <row r="11">
@@ -891,7 +1051,22 @@
         <v>28</v>
       </c>
       <c r="N11" t="n">
-        <v>334</v>
+        <v>24</v>
+      </c>
+      <c r="O11" t="n">
+        <v>28</v>
+      </c>
+      <c r="P11" t="n">
+        <v>26</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>31</v>
+      </c>
+      <c r="R11" t="n">
+        <v>6</v>
+      </c>
+      <c r="S11" t="n">
+        <v>449</v>
       </c>
     </row>
     <row r="12">
@@ -937,7 +1112,22 @@
         <v>28</v>
       </c>
       <c r="N12" t="n">
-        <v>324</v>
+        <v>32</v>
+      </c>
+      <c r="O12" t="n">
+        <v>37</v>
+      </c>
+      <c r="P12" t="n">
+        <v>31</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>29</v>
+      </c>
+      <c r="R12" t="n">
+        <v>6</v>
+      </c>
+      <c r="S12" t="n">
+        <v>459</v>
       </c>
     </row>
     <row r="13">
@@ -983,7 +1173,22 @@
         <v>32</v>
       </c>
       <c r="N13" t="n">
-        <v>370</v>
+        <v>29</v>
+      </c>
+      <c r="O13" t="n">
+        <v>29</v>
+      </c>
+      <c r="P13" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>34</v>
+      </c>
+      <c r="R13" t="n">
+        <v>7</v>
+      </c>
+      <c r="S13" t="n">
+        <v>499</v>
       </c>
     </row>
     <row r="14">
@@ -1029,7 +1234,22 @@
         <v>31</v>
       </c>
       <c r="N14" t="n">
-        <v>339</v>
+        <v>25</v>
+      </c>
+      <c r="O14" t="n">
+        <v>22</v>
+      </c>
+      <c r="P14" t="n">
+        <v>17</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>26</v>
+      </c>
+      <c r="R14" t="n">
+        <v>4</v>
+      </c>
+      <c r="S14" t="n">
+        <v>433</v>
       </c>
     </row>
     <row r="15">
@@ -1075,7 +1295,22 @@
         <v>26</v>
       </c>
       <c r="N15" t="n">
-        <v>340</v>
+        <v>24</v>
+      </c>
+      <c r="O15" t="n">
+        <v>25</v>
+      </c>
+      <c r="P15" t="n">
+        <v>27</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>26</v>
+      </c>
+      <c r="R15" t="n">
+        <v>4</v>
+      </c>
+      <c r="S15" t="n">
+        <v>446</v>
       </c>
     </row>
   </sheetData>
@@ -1089,7 +1324,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N15"/>
+  <dimension ref="A1:S15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1160,6 +1395,31 @@
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
+          <t>Week13</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Week14</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Week15</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Week16</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Week17</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
           <t>Total</t>
         </is>
       </c>
@@ -1207,467 +1467,632 @@
         <v>21</v>
       </c>
       <c r="N2" t="n">
-        <v>308</v>
+        <v>21</v>
+      </c>
+      <c r="O2" t="n">
+        <v>25</v>
+      </c>
+      <c r="P2" t="n">
+        <v>16</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>15</v>
+      </c>
+      <c r="R2" t="n">
+        <v>2</v>
+      </c>
+      <c r="S2" t="n">
+        <v>387</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>abass</t>
+          <t>jordanc</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C3" t="n">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D3" t="n">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E3" t="n">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F3" t="n">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="G3" t="n">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H3" t="n">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="I3" t="n">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="J3" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K3" t="n">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="L3" t="n">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="M3" t="n">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="N3" t="n">
-        <v>324</v>
+        <v>25</v>
+      </c>
+      <c r="O3" t="n">
+        <v>22</v>
+      </c>
+      <c r="P3" t="n">
+        <v>17</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>26</v>
+      </c>
+      <c r="R3" t="n">
+        <v>4</v>
+      </c>
+      <c r="S3" t="n">
+        <v>433</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>zach</t>
+          <t>hurley</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C4" t="n">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D4" t="n">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E4" t="n">
         <v>30</v>
       </c>
       <c r="F4" t="n">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="G4" t="n">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="H4" t="n">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="I4" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="J4" t="n">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="K4" t="n">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="L4" t="n">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="M4" t="n">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="N4" t="n">
-        <v>334</v>
+        <v>24</v>
+      </c>
+      <c r="O4" t="n">
+        <v>25</v>
+      </c>
+      <c r="P4" t="n">
+        <v>27</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>26</v>
+      </c>
+      <c r="R4" t="n">
+        <v>4</v>
+      </c>
+      <c r="S4" t="n">
+        <v>446</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>jordanc</t>
+          <t>zach</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C5" t="n">
         <v>33</v>
       </c>
       <c r="D5" t="n">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E5" t="n">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F5" t="n">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="G5" t="n">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="H5" t="n">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="I5" t="n">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="J5" t="n">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="K5" t="n">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="L5" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="M5" t="n">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="N5" t="n">
-        <v>339</v>
+        <v>24</v>
+      </c>
+      <c r="O5" t="n">
+        <v>28</v>
+      </c>
+      <c r="P5" t="n">
+        <v>26</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>31</v>
+      </c>
+      <c r="R5" t="n">
+        <v>6</v>
+      </c>
+      <c r="S5" t="n">
+        <v>449</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>hurley</t>
+          <t>abass</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C6" t="n">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D6" t="n">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="E6" t="n">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F6" t="n">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G6" t="n">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H6" t="n">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="I6" t="n">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J6" t="n">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="K6" t="n">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="L6" t="n">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="M6" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="N6" t="n">
-        <v>340</v>
+        <v>32</v>
+      </c>
+      <c r="O6" t="n">
+        <v>37</v>
+      </c>
+      <c r="P6" t="n">
+        <v>31</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>29</v>
+      </c>
+      <c r="R6" t="n">
+        <v>6</v>
+      </c>
+      <c r="S6" t="n">
+        <v>459</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>rico</t>
+          <t>kenneth</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="C7" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D7" t="n">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E7" t="n">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F7" t="n">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="G7" t="n">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H7" t="n">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="I7" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="J7" t="n">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="K7" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L7" t="n">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="M7" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="N7" t="n">
-        <v>352</v>
+        <v>27</v>
+      </c>
+      <c r="O7" t="n">
+        <v>31</v>
+      </c>
+      <c r="P7" t="n">
+        <v>22</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>32</v>
+      </c>
+      <c r="R7" t="n">
+        <v>3</v>
+      </c>
+      <c r="S7" t="n">
+        <v>472</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>kenneth</t>
+          <t>rico</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="C8" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D8" t="n">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E8" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F8" t="n">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="G8" t="n">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H8" t="n">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="I8" t="n">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="J8" t="n">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="K8" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L8" t="n">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="M8" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N8" t="n">
-        <v>357</v>
+        <v>32</v>
+      </c>
+      <c r="O8" t="n">
+        <v>32</v>
+      </c>
+      <c r="P8" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>26</v>
+      </c>
+      <c r="R8" t="n">
+        <v>6</v>
+      </c>
+      <c r="S8" t="n">
+        <v>478</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>spencer</t>
+          <t>ned</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C9" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D9" t="n">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="E9" t="n">
         <v>33</v>
       </c>
       <c r="F9" t="n">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="G9" t="n">
         <v>33</v>
       </c>
       <c r="H9" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I9" t="n">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="J9" t="n">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="K9" t="n">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L9" t="n">
         <v>29</v>
       </c>
       <c r="M9" t="n">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="N9" t="n">
-        <v>359</v>
+        <v>29</v>
+      </c>
+      <c r="O9" t="n">
+        <v>33</v>
+      </c>
+      <c r="P9" t="n">
+        <v>26</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>26</v>
+      </c>
+      <c r="R9" t="n">
+        <v>6</v>
+      </c>
+      <c r="S9" t="n">
+        <v>481</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>yinka</t>
+          <t>lamin</t>
         </is>
       </c>
       <c r="B10" t="n">
+        <v>25</v>
+      </c>
+      <c r="C10" t="n">
+        <v>35</v>
+      </c>
+      <c r="D10" t="n">
+        <v>32</v>
+      </c>
+      <c r="E10" t="n">
+        <v>28</v>
+      </c>
+      <c r="F10" t="n">
+        <v>29</v>
+      </c>
+      <c r="G10" t="n">
+        <v>34</v>
+      </c>
+      <c r="H10" t="n">
+        <v>32</v>
+      </c>
+      <c r="I10" t="n">
+        <v>34</v>
+      </c>
+      <c r="J10" t="n">
+        <v>32</v>
+      </c>
+      <c r="K10" t="n">
+        <v>30</v>
+      </c>
+      <c r="L10" t="n">
+        <v>30</v>
+      </c>
+      <c r="M10" t="n">
+        <v>29</v>
+      </c>
+      <c r="N10" t="n">
         <v>24</v>
       </c>
-      <c r="C10" t="n">
-        <v>29</v>
-      </c>
-      <c r="D10" t="n">
-        <v>30</v>
-      </c>
-      <c r="E10" t="n">
-        <v>27</v>
-      </c>
-      <c r="F10" t="n">
-        <v>32</v>
-      </c>
-      <c r="G10" t="n">
-        <v>34</v>
-      </c>
-      <c r="H10" t="n">
-        <v>30</v>
-      </c>
-      <c r="I10" t="n">
-        <v>35</v>
-      </c>
-      <c r="J10" t="n">
-        <v>29</v>
-      </c>
-      <c r="K10" t="n">
-        <v>31</v>
-      </c>
-      <c r="L10" t="n">
-        <v>24</v>
-      </c>
-      <c r="M10" t="n">
-        <v>35</v>
-      </c>
-      <c r="N10" t="n">
-        <v>360</v>
+      <c r="O10" t="n">
+        <v>30</v>
+      </c>
+      <c r="P10" t="n">
+        <v>26</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>31</v>
+      </c>
+      <c r="R10" t="n">
+        <v>7</v>
+      </c>
+      <c r="S10" t="n">
+        <v>488</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>ned</t>
+          <t>yinka</t>
         </is>
       </c>
       <c r="B11" t="n">
         <v>24</v>
       </c>
       <c r="C11" t="n">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D11" t="n">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E11" t="n">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F11" t="n">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="G11" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H11" t="n">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I11" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="J11" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K11" t="n">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="L11" t="n">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="M11" t="n">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="N11" t="n">
-        <v>361</v>
+        <v>31</v>
+      </c>
+      <c r="O11" t="n">
+        <v>35</v>
+      </c>
+      <c r="P11" t="n">
+        <v>28</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>28</v>
+      </c>
+      <c r="R11" t="n">
+        <v>6</v>
+      </c>
+      <c r="S11" t="n">
+        <v>488</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>lamin</t>
+          <t>spencer</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C12" t="n">
+        <v>31</v>
+      </c>
+      <c r="D12" t="n">
+        <v>26</v>
+      </c>
+      <c r="E12" t="n">
+        <v>33</v>
+      </c>
+      <c r="F12" t="n">
+        <v>32</v>
+      </c>
+      <c r="G12" t="n">
+        <v>33</v>
+      </c>
+      <c r="H12" t="n">
+        <v>31</v>
+      </c>
+      <c r="I12" t="n">
         <v>35</v>
       </c>
-      <c r="D12" t="n">
-        <v>32</v>
-      </c>
-      <c r="E12" t="n">
-        <v>28</v>
-      </c>
-      <c r="F12" t="n">
-        <v>29</v>
-      </c>
-      <c r="G12" t="n">
-        <v>34</v>
-      </c>
-      <c r="H12" t="n">
-        <v>32</v>
-      </c>
-      <c r="I12" t="n">
-        <v>34</v>
-      </c>
       <c r="J12" t="n">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K12" t="n">
         <v>30</v>
       </c>
       <c r="L12" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M12" t="n">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="N12" t="n">
-        <v>370</v>
+        <v>34</v>
+      </c>
+      <c r="O12" t="n">
+        <v>39</v>
+      </c>
+      <c r="P12" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>28</v>
+      </c>
+      <c r="R12" t="n">
+        <v>4</v>
+      </c>
+      <c r="S12" t="n">
+        <v>497</v>
       </c>
     </row>
     <row r="13">
@@ -1713,99 +2138,144 @@
         <v>32</v>
       </c>
       <c r="N13" t="n">
-        <v>370</v>
+        <v>29</v>
+      </c>
+      <c r="O13" t="n">
+        <v>29</v>
+      </c>
+      <c r="P13" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>34</v>
+      </c>
+      <c r="R13" t="n">
+        <v>7</v>
+      </c>
+      <c r="S13" t="n">
+        <v>499</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>narayan</t>
+          <t>miles</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C14" t="n">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="D14" t="n">
         <v>31</v>
       </c>
       <c r="E14" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F14" t="n">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G14" t="n">
         <v>34</v>
       </c>
       <c r="H14" t="n">
+        <v>34</v>
+      </c>
+      <c r="I14" t="n">
         <v>38</v>
       </c>
-      <c r="I14" t="n">
-        <v>33</v>
-      </c>
       <c r="J14" t="n">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="K14" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L14" t="n">
         <v>32</v>
       </c>
       <c r="M14" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="N14" t="n">
-        <v>388</v>
+        <v>33</v>
+      </c>
+      <c r="O14" t="n">
+        <v>34</v>
+      </c>
+      <c r="P14" t="n">
+        <v>27</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>34</v>
+      </c>
+      <c r="R14" t="n">
+        <v>5</v>
+      </c>
+      <c r="S14" t="n">
+        <v>522</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>miles</t>
+          <t>narayan</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C15" t="n">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D15" t="n">
         <v>31</v>
       </c>
       <c r="E15" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F15" t="n">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G15" t="n">
         <v>34</v>
       </c>
       <c r="H15" t="n">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="I15" t="n">
+        <v>33</v>
+      </c>
+      <c r="J15" t="n">
+        <v>34</v>
+      </c>
+      <c r="K15" t="n">
+        <v>28</v>
+      </c>
+      <c r="L15" t="n">
+        <v>32</v>
+      </c>
+      <c r="M15" t="n">
+        <v>33</v>
+      </c>
+      <c r="N15" t="n">
+        <v>33</v>
+      </c>
+      <c r="O15" t="n">
+        <v>33</v>
+      </c>
+      <c r="P15" t="n">
+        <v>26</v>
+      </c>
+      <c r="Q15" t="n">
         <v>38</v>
       </c>
-      <c r="J15" t="n">
-        <v>30</v>
-      </c>
-      <c r="K15" t="n">
-        <v>30</v>
-      </c>
-      <c r="L15" t="n">
-        <v>32</v>
-      </c>
-      <c r="M15" t="n">
-        <v>34</v>
-      </c>
-      <c r="N15" t="n">
-        <v>389</v>
+      <c r="R15" t="n">
+        <v>4</v>
+      </c>
+      <c r="S15" t="n">
+        <v>522</v>
       </c>
     </row>
   </sheetData>

</xml_diff>